<commit_message>
desagregar los datos de de metas, subir archivos planos para catalogo
</commit_message>
<xml_diff>
--- a/Archivos/2020_IMPORTARC_9536_10000000.xlsx
+++ b/Archivos/2020_IMPORTARC_9536_10000000.xlsx
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>